<commit_message>
Added sour patch data from Rachel.
</commit_message>
<xml_diff>
--- a/ScienceSaturday07/raw_data.xlsx
+++ b/ScienceSaturday07/raw_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dr1015bob/temp/ScienceSaturday/ScienceSaturday07/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AA6789-457E-A54A-9F40-7AEB3987D2C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D4D03D-635E-414E-80D8-6756DCCE284F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="173">
   <si>
     <t>Guesser</t>
   </si>
@@ -534,13 +534,31 @@
   </si>
   <si>
     <t>not confident</t>
+  </si>
+  <si>
+    <t>Sour patch kids</t>
+  </si>
+  <si>
+    <t>if red is an option then it's red</t>
+  </si>
+  <si>
+    <t>water break. let me pour myself more rum</t>
+  </si>
+  <si>
+    <t>idk it didn't really taste like anything</t>
+  </si>
+  <si>
+    <t>for sure, if it's not orange then i screwed up</t>
+  </si>
+  <si>
+    <t>torn between yellow and green</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -590,8 +608,21 @@
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -670,6 +701,12 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF40FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -698,7 +735,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -860,12 +897,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF40FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -5311,9 +5355,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -5327,7 +5373,7 @@
     <col min="9" max="9" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -5335,7 +5381,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1">
       <c r="A2" s="47" t="s">
         <v>1</v>
       </c>
@@ -5343,10 +5389,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1">
+    <row r="3" spans="1:13" ht="15.75" customHeight="1">
       <c r="A3" s="28"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1">
       <c r="A4" s="49" t="s">
         <v>2</v>
       </c>
@@ -5362,8 +5408,14 @@
       <c r="G4" s="52"/>
       <c r="H4" s="52"/>
       <c r="I4" s="52"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1">
+      <c r="J4" s="107" t="s">
+        <v>167</v>
+      </c>
+      <c r="K4" s="107"/>
+      <c r="L4" s="107"/>
+      <c r="M4" s="107"/>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" customHeight="1">
       <c r="A5" s="49" t="s">
         <v>9</v>
       </c>
@@ -5381,8 +5433,14 @@
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="55"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1">
+      <c r="J5" s="107">
+        <v>4</v>
+      </c>
+      <c r="K5" s="107"/>
+      <c r="L5" s="107"/>
+      <c r="M5" s="107"/>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" customHeight="1">
       <c r="A6" s="49" t="s">
         <v>10</v>
       </c>
@@ -5410,8 +5468,20 @@
       <c r="I6" s="58" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1">
+      <c r="J6" s="108" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="108" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="108" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" s="108" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" customHeight="1">
       <c r="A7" s="60">
         <v>1</v>
       </c>
@@ -5437,8 +5507,18 @@
         <v>1</v>
       </c>
       <c r="I7" s="55"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1">
+      <c r="J7" s="107" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="107" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="107" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7" s="107"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1">
       <c r="A8" s="60">
         <v>2</v>
       </c>
@@ -5466,8 +5546,18 @@
         <v>1</v>
       </c>
       <c r="I8" s="55"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1">
+      <c r="J8" s="107" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" s="107" t="s">
+        <v>65</v>
+      </c>
+      <c r="L8" s="107" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" s="107"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" customHeight="1">
       <c r="A9" s="60">
         <v>3</v>
       </c>
@@ -5495,8 +5585,20 @@
       <c r="I9" s="54" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1">
+      <c r="J9" s="107" t="s">
+        <v>68</v>
+      </c>
+      <c r="K9" s="107" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="107" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9" s="107" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" customHeight="1">
       <c r="A10" s="60">
         <v>4</v>
       </c>
@@ -5524,8 +5626,20 @@
       <c r="I10" s="54" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1">
+      <c r="J10" s="107" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="107" t="s">
+        <v>66</v>
+      </c>
+      <c r="L10" s="107" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" s="107" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" customHeight="1">
       <c r="A11" s="60">
         <v>5</v>
       </c>
@@ -5551,8 +5665,18 @@
         <v>1</v>
       </c>
       <c r="I11" s="55"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1">
+      <c r="J11" s="107" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="107" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11" s="107" t="b">
+        <v>0</v>
+      </c>
+      <c r="M11" s="107"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" customHeight="1">
       <c r="A12" s="60">
         <v>6</v>
       </c>
@@ -5578,8 +5702,18 @@
         <v>1</v>
       </c>
       <c r="I12" s="55"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1">
+      <c r="J12" s="107" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="107" t="s">
+        <v>65</v>
+      </c>
+      <c r="L12" s="107" t="b">
+        <v>0</v>
+      </c>
+      <c r="M12" s="107"/>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" customHeight="1">
       <c r="A13" s="60">
         <v>7</v>
       </c>
@@ -5607,8 +5741,20 @@
         <v>1</v>
       </c>
       <c r="I13" s="55"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1">
+      <c r="J13" s="107" t="s">
+        <v>65</v>
+      </c>
+      <c r="K13" s="107" t="s">
+        <v>66</v>
+      </c>
+      <c r="L13" s="107" t="b">
+        <v>0</v>
+      </c>
+      <c r="M13" s="107" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" customHeight="1">
       <c r="A14" s="60">
         <v>8</v>
       </c>
@@ -5638,8 +5784,18 @@
       <c r="I14" s="54" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1">
+      <c r="J14" s="107" t="s">
+        <v>68</v>
+      </c>
+      <c r="K14" s="107" t="s">
+        <v>68</v>
+      </c>
+      <c r="L14" s="107" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" s="107"/>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" customHeight="1">
       <c r="A15" s="60">
         <v>9</v>
       </c>
@@ -5665,8 +5821,18 @@
         <v>1</v>
       </c>
       <c r="I15" s="55"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1">
+      <c r="J15" s="107" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15" s="107" t="s">
+        <v>65</v>
+      </c>
+      <c r="L15" s="107" t="b">
+        <v>1</v>
+      </c>
+      <c r="M15" s="107"/>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" customHeight="1">
       <c r="A16" s="60">
         <v>10</v>
       </c>
@@ -5692,8 +5858,20 @@
         <v>1</v>
       </c>
       <c r="I16" s="55"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1">
+      <c r="J16" s="107" t="s">
+        <v>66</v>
+      </c>
+      <c r="K16" s="107" t="s">
+        <v>66</v>
+      </c>
+      <c r="L16" s="107" t="b">
+        <v>1</v>
+      </c>
+      <c r="M16" s="107" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" customHeight="1">
       <c r="A17" s="60">
         <v>11</v>
       </c>
@@ -5719,8 +5897,18 @@
         <v>1</v>
       </c>
       <c r="I17" s="55"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1">
+      <c r="J17" s="107" t="s">
+        <v>66</v>
+      </c>
+      <c r="K17" s="107" t="s">
+        <v>66</v>
+      </c>
+      <c r="L17" s="107" t="b">
+        <v>1</v>
+      </c>
+      <c r="M17" s="107"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" customHeight="1">
       <c r="A18" s="60">
         <v>12</v>
       </c>
@@ -5748,8 +5936,18 @@
         <v>1</v>
       </c>
       <c r="I18" s="55"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1">
+      <c r="J18" s="107" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" s="107" t="s">
+        <v>68</v>
+      </c>
+      <c r="L18" s="107" t="b">
+        <v>0</v>
+      </c>
+      <c r="M18" s="107"/>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" customHeight="1">
       <c r="A19" s="60">
         <v>13</v>
       </c>
@@ -5775,8 +5973,18 @@
         <v>1</v>
       </c>
       <c r="I19" s="55"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1">
+      <c r="J19" s="107" t="s">
+        <v>66</v>
+      </c>
+      <c r="K19" s="107" t="s">
+        <v>66</v>
+      </c>
+      <c r="L19" s="107" t="b">
+        <v>1</v>
+      </c>
+      <c r="M19" s="107"/>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" customHeight="1">
       <c r="A20" s="60">
         <v>14</v>
       </c>
@@ -5802,8 +6010,20 @@
         <v>1</v>
       </c>
       <c r="I20" s="55"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1">
+      <c r="J20" s="107" t="s">
+        <v>65</v>
+      </c>
+      <c r="K20" s="107" t="s">
+        <v>65</v>
+      </c>
+      <c r="L20" s="107" t="b">
+        <v>1</v>
+      </c>
+      <c r="M20" s="107" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" customHeight="1">
       <c r="A21" s="60">
         <v>15</v>
       </c>
@@ -5829,12 +6049,22 @@
         <v>0</v>
       </c>
       <c r="I21" s="55"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1">
+      <c r="J21" s="107" t="s">
+        <v>68</v>
+      </c>
+      <c r="K21" s="107" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" s="107" t="b">
+        <v>0</v>
+      </c>
+      <c r="M21" s="107"/>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" customHeight="1">
       <c r="D22" s="63"/>
       <c r="H22" s="63"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1">
+    <row r="23" spans="1:13" ht="15.75" customHeight="1">
       <c r="B23" s="48" t="s">
         <v>56</v>
       </c>
@@ -5847,7 +6077,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1">
+    <row r="24" spans="1:13" ht="15.75" customHeight="1">
       <c r="B24" s="48" t="s">
         <v>57</v>
       </c>
@@ -5860,32 +6090,32 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1">
+    <row r="25" spans="1:13" ht="15.75" customHeight="1">
       <c r="B25" s="48" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1">
+    <row r="26" spans="1:13" ht="15.75" customHeight="1">
       <c r="B26" s="48" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1">
+    <row r="27" spans="1:13" ht="15.75" customHeight="1">
       <c r="B27" s="48" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1">
+    <row r="28" spans="1:13" ht="15.75" customHeight="1">
       <c r="B28" s="48" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1">
+    <row r="29" spans="1:13" ht="15.75" customHeight="1">
       <c r="B29" s="48" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1">
+    <row r="30" spans="1:13" ht="15.75" customHeight="1">
       <c r="B30" s="65">
         <f>(52/65) *(51/65)*(50/65)*(49/65)*(48/65)*(47/65)*(46/65)*(45/65)*(44/65)*(43/65)*(42/65)*(41/65)*(40/65)*(39/65)*(38/65)</f>
         <v>3.7515537174951856E-3</v>
@@ -9475,7 +9705,7 @@
   </sheetPr>
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>

</xml_diff>